<commit_message>
Última versión de la limpieza y preparación de datos
</commit_message>
<xml_diff>
--- a/ARIMA.xlsx
+++ b/ARIMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA48794-6ADC-44AC-A1EC-806EF98080B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3863B194-BFED-4139-93AC-C71F1D9CFE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1EFCCBE9-0A00-4D72-A1ED-25141A2F4EC5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>3,0,0</t>
   </si>
@@ -113,12 +113,6 @@
     <t>07 - Delitos</t>
   </si>
   <si>
-    <t>08 - Retail</t>
-  </si>
-  <si>
-    <t>08 - Restaurantes</t>
-  </si>
-  <si>
     <t>09 - Vivienda</t>
   </si>
   <si>
@@ -141,6 +135,9 @@
   </si>
   <si>
     <t>Sutton</t>
+  </si>
+  <si>
+    <t>08 - Servicios</t>
   </si>
 </sst>
 </file>
@@ -209,18 +206,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7A067C-4247-4426-BBA1-9A3ACDDDDC04}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,10 +563,10 @@
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -596,19 +592,16 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -619,13 +612,10 @@
         <v>2</v>
       </c>
       <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -636,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -658,20 +648,17 @@
       <c r="I4">
         <v>28</v>
       </c>
-      <c r="J4">
-        <v>8</v>
+      <c r="J4" s="2">
+        <v>23</v>
       </c>
       <c r="K4">
         <v>11</v>
       </c>
       <c r="L4">
-        <v>11</v>
-      </c>
-      <c r="M4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -684,23 +671,20 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>15</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
         <v>14</v>
       </c>
-      <c r="K5" s="5">
-        <v>16</v>
-      </c>
-      <c r="L5" s="5">
-        <v>14</v>
-      </c>
-      <c r="M5" s="6">
+      <c r="L5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -708,24 +692,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>9</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -739,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -747,50 +731,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>8</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>10</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>7</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11">
         <v>4</v>
       </c>
       <c r="J11" s="3">
         <v>4</v>
       </c>
-      <c r="K11" s="3">
-        <v>4</v>
-      </c>
-      <c r="L11">
+      <c r="K11">
         <v>8</v>
       </c>
-      <c r="M11" s="3">
+      <c r="L11" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -798,7 +779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -806,11 +787,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>10</v>
       </c>
       <c r="C14">
@@ -820,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -830,11 +811,8 @@
       <c r="F15">
         <v>2</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -842,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -858,57 +836,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="7">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
         <f>SUM(B2:B18)</f>
         <v>33</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <f>SUM(C2:C18)</f>
         <v>33</v>
       </c>
-      <c r="D19" s="7">
-        <f t="shared" ref="D19:N19" si="0">SUM(D2:D18)</f>
+      <c r="D19" s="5">
+        <f t="shared" ref="D19:L19" si="0">SUM(D2:D18)</f>
         <v>33</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="L19" s="7">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="M19" s="7">
+      <c r="L19" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>1</v>
       </c>
@@ -916,33 +890,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
         <v>30</v>
       </c>
-      <c r="H21" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" t="s">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
         <v>31</v>
       </c>
-      <c r="K21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J22" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J24" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>